<commit_message>
Orsha Report update. Restore alfabet sorting. Added out certificates to report
</commit_message>
<xml_diff>
--- a/CCICertificate/WebContent/resources/in/ReportOrsha.xlsx
+++ b/CCICertificate/WebContent/resources/in/ReportOrsha.xlsx
@@ -8,16 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Out" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Реестр сертификатов продукции (работ, услуг) собственного производства, выданных юридическим лицам и индивидуальным предпринимателям, зарегистрированным в Республике Беларусь с местом нахождения (жительства) в Оршанском районе</t>
   </si>
@@ -50,13 +49,40 @@
   </si>
   <si>
     <t xml:space="preserve">Место производства продукции (работ, услуг) </t>
+  </si>
+  <si>
+    <t>№ п.п.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Производитель продукции                                   (место производства - вне Оршанского района)                         </t>
+  </si>
+  <si>
+    <t>Дата выдачи сертификата</t>
+  </si>
+  <si>
+    <t>Номера сертификата</t>
+  </si>
+  <si>
+    <t>Форма сертификата</t>
+  </si>
+  <si>
+    <t>Укрупненное наименование продукции собственного производства</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Место нахождения производства: для продукции - на основании информации, указанной в сертификате; для работ, услуг - на основании информации в заявлении заказчика на экспертизу </t>
+  </si>
+  <si>
+    <t xml:space="preserve">до  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Реестр сертификатов продукции  собственного производства, выданных юридическим лицам и индивидуальным предпринимателям, зарегистрированным в Республике Беларусь с местом нахождения (жительства) в Оршанском районе и местом производства вне Оршанского района </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +112,13 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -101,7 +134,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -172,11 +205,87 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -187,6 +296,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -199,13 +314,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -555,59 +697,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="103.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="86.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -628,13 +770,92 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="46.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="20"/>
+      <c r="G2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:G3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>